<commit_message>
agregar campos producto, precio_unitario, total_venta
</commit_message>
<xml_diff>
--- a/Analisis de venta y rendimiento comercial/analisis_ventas.xlsx
+++ b/Analisis de venta y rendimiento comercial/analisis_ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jbernal\Excel_Projects\Analisis de venta y rendimiento comercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DBE0FA-2200-4085-8081-A55692477599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2BFA2D-3179-435D-9071-FFC9C4996235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{C3689989-C428-4383-B478-D0EDFC37C904}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C3689989-C428-4383-B478-D0EDFC37C904}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Crudos" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>ID_Venta</t>
   </si>
@@ -193,7 +193,39 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -204,6 +236,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A92B6507-4B6A-4B49-B413-87F7A39C07E3}" name="tbl_Productos" displayName="tbl_Productos" ref="A1:C5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:C5" xr:uid="{A92B6507-4B6A-4B49-B413-87F7A39C07E3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C55A325D-7BD6-49AC-B11E-EDF0A27B1C16}" name="Producto" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A0FFE583-A718-487D-81FE-9C07633F39F7}" name="Categoría" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{9177BD52-4EA4-494A-BEA0-D32F3FBB1A94}" name="Precio_Unitario" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,20 +746,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D223AA19-3F82-4913-9D8A-B900C901E1CA}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,16 +786,22 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1001</v>
       </c>
@@ -775,8 +826,19 @@
       <c r="H2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2">
+        <f>VLOOKUP(I2,tbl_Productos[],3,)</f>
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <f>H2*J2</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1002</v>
       </c>
@@ -799,10 +861,21 @@
         <v>14</v>
       </c>
       <c r="H3" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2">
+        <f>VLOOKUP(I3,tbl_Productos[],3,)</f>
+        <v>2500</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K6" si="0">H3*J3</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1003</v>
       </c>
@@ -825,10 +898,21 @@
         <v>11</v>
       </c>
       <c r="H4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="2">
+        <f>VLOOKUP(I4,tbl_Productos[],3,)</f>
+        <v>900</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1004</v>
       </c>
@@ -851,10 +935,21 @@
         <v>14</v>
       </c>
       <c r="H5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="2">
+        <f>VLOOKUP(I5,tbl_Productos[],3,)</f>
+        <v>900</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1005</v>
       </c>
@@ -877,11 +972,40 @@
         <v>11</v>
       </c>
       <c r="H6" s="2">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="2">
+        <f>VLOOKUP(I6,tbl_Productos[],3,)</f>
+        <v>300</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>4800</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{56A338E2-FAA5-4BDE-8A62-271F32D614C1}">
+      <formula1>1</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5866A43A-292A-423D-A39B-46379CB8812C}">
+          <x14:formula1>
+            <xm:f>Productos!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -889,13 +1013,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA35C4B-DD2E-420C-9957-486FA74CFD36}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -955,5 +1080,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ventas de tecnologia en bogota
</commit_message>
<xml_diff>
--- a/Analisis de venta y rendimiento comercial/analisis_ventas.xlsx
+++ b/Analisis de venta y rendimiento comercial/analisis_ventas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jbernal\Excel_Projects\Analisis de venta y rendimiento comercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989FCBD-A807-4ECC-858B-24F8C8523A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE6B908-3E48-4F07-91A4-21A459EAE4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{C3689989-C428-4383-B478-D0EDFC37C904}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
   <si>
     <t>ID_Venta</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Meta</t>
+  </si>
+  <si>
+    <t>Ventas de Tecnologia en Bogota</t>
   </si>
 </sst>
 </file>
@@ -951,7 +954,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,19 +1147,19 @@
         <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" t="str">
         <f>INDEX(tbl_Productos[Categoría],MATCH(H4,tbl_Productos[Producto],0))</f>
-        <v>Muebles</v>
+        <v>Tecnología</v>
       </c>
       <c r="J4" s="2">
         <f>VLOOKUP(H4,tbl_Productos[],3,)</f>
-        <v>900</v>
+        <v>2500</v>
       </c>
       <c r="K4">
         <f>G4*J4</f>
-        <v>21600</v>
+        <v>60000</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
@@ -1164,7 +1167,7 @@
       </c>
       <c r="M4">
         <f>K4*INDEX(tbl_Comisiones[PCT_comision],MATCH(I4,tbl_Comisiones[Categoria],0))</f>
-        <v>1944</v>
+        <v>3600</v>
       </c>
       <c r="N4" t="str">
         <f>INDEX(tbl_vendedores[Zona],MATCH(D4,tbl_vendedores[Vendedor],0))</f>
@@ -1537,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44D6B31-8C4D-400A-89C4-83AC6B681457}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1568,7 @@
       </c>
       <c r="B2" s="2">
         <f>SUM(tbl_Ventas[Total_Ventas])</f>
-        <v>42900</v>
+        <v>81300</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -1595,25 +1598,25 @@
       </c>
       <c r="B3" s="2">
         <f>SUM(tbl_Ventas[Comision])</f>
-        <v>3636</v>
+        <v>5292</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2">
         <f>SUMIF(tbl_Ventas[Categoria],E3,tbl_Ventas[Total_Ventas])</f>
-        <v>7500</v>
+        <v>67500</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
       </c>
       <c r="J3">
         <f>SUMIF(tbl_Ventas[Vendedor],I3,tbl_Ventas[Total_Ventas])</f>
-        <v>28200</v>
+        <v>66600</v>
       </c>
       <c r="K3">
         <f>SUMIF(tbl_Ventas[Vendedor],I3,tbl_Ventas[Comision])</f>
-        <v>2538</v>
+        <v>4194</v>
       </c>
       <c r="L3">
         <f>HLOOKUP(I3,Catalogos!$E$1:$H$2,2,FALSE)</f>
@@ -1637,7 +1640,7 @@
       </c>
       <c r="F4" s="2">
         <f>SUMIF(tbl_Ventas[Categoria],E4,tbl_Ventas[Total_Ventas])</f>
-        <v>35400</v>
+        <v>13800</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -1665,7 +1668,7 @@
       </c>
       <c r="B5" s="2">
         <f>AVERAGE(tbl_Ventas[Total_Ventas])</f>
-        <v>8580</v>
+        <v>16260</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
@@ -1685,6 +1688,17 @@
       <c r="M5" t="str">
         <f t="shared" si="0"/>
         <v>No Cumple</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>SUMIFS(tbl_Ventas[Total_Ventas],tbl_Ventas[Categoria],"Tecnología",tbl_Ventas[Ciudad_Cliente],"Bogotá")</f>
+        <v>60000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregar datos y actualizar
</commit_message>
<xml_diff>
--- a/Analisis de venta y rendimiento comercial/analisis_ventas.xlsx
+++ b/Analisis de venta y rendimiento comercial/analisis_ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jbernal\Excel_Projects\Analisis de venta y rendimiento comercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB281B0-2132-4F91-9796-AB15AA12BD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09895147-1F98-4490-AF5C-4FEFA42E82BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{C3689989-C428-4383-B478-D0EDFC37C904}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{C3689989-C428-4383-B478-D0EDFC37C904}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Crudos" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId8"/>
+    <pivotCache cacheId="13" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>ID_Venta</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Suma de Margen</t>
+  </si>
+  <si>
+    <t>Daniel Saenz</t>
   </si>
 </sst>
 </file>
@@ -2160,13 +2163,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeinfferson B" refreshedDate="46062.543981712966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="5" xr:uid="{BD0C2A9B-79B2-47CB-A8E6-DE14BF5EA00E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeinfferson B" refreshedDate="46062.581010532405" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="6" xr:uid="{BD0C2A9B-79B2-47CB-A8E6-DE14BF5EA00E}">
   <cacheSource type="worksheet">
     <worksheetSource name="tbl_Ventas"/>
   </cacheSource>
   <cacheFields count="15">
     <cacheField name="Fecha" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2024-01-05T00:00:00" maxDate="2024-01-09T00:00:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2024-01-05T00:00:00" maxDate="2024-01-10T00:00:00"/>
     </cacheField>
     <cacheField name="Nombre_Cliente" numFmtId="49">
       <sharedItems/>
@@ -2229,7 +2232,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="5">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="6">
   <r>
     <d v="2024-01-05T00:00:00"/>
     <s v="Ana Gómez "/>
@@ -2310,11 +2313,27 @@
     <s v="Centro"/>
     <n v="15000"/>
   </r>
+  <r>
+    <d v="2024-01-09T00:00:00"/>
+    <s v="Daniel Saenz"/>
+    <s v="Diana"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3"/>
+    <s v="Laptop"/>
+    <x v="1"/>
+    <n v="2500"/>
+    <n v="7500"/>
+    <s v="Alta"/>
+    <n v="450"/>
+    <s v="Norte"/>
+    <n v="12000"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1D9401C-0867-4023-8396-216647198446}" name="TablaDinámica1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1D9401C-0867-4023-8396-216647198446}" name="TablaDinámica1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:G7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField numFmtId="14" showAll="0"/>
@@ -2557,8 +2576,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D6F5F690-9516-436E-95BD-879E016B9934}" name="tbl_Ventas" displayName="tbl_Ventas" ref="B1:O6" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="B1:O6" xr:uid="{D6F5F690-9516-436E-95BD-879E016B9934}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D6F5F690-9516-436E-95BD-879E016B9934}" name="tbl_Ventas" displayName="tbl_Ventas" ref="B1:O7" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="B1:O7" xr:uid="{D6F5F690-9516-436E-95BD-879E016B9934}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{F686120E-3EBE-4819-A4C9-C5C19E7694D8}" name="Fecha" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{57EC154B-AFCA-4F28-B2A5-1B3D4A522B8B}" name="Nombre_Cliente" dataDxfId="17"/>
@@ -3133,10 +3152,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D223AA19-3F82-4913-9D8A-B900C901E1CA}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3468,9 +3487,63 @@
         <v>15000</v>
       </c>
     </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1006</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45300</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="str">
+        <f>INDEX(tbl_Productos[Categoría],MATCH(H7,tbl_Productos[Producto],0))</f>
+        <v>Tecnología</v>
+      </c>
+      <c r="J7" s="2">
+        <f>VLOOKUP(H7,tbl_Productos[],3,)</f>
+        <v>2500</v>
+      </c>
+      <c r="K7">
+        <f>G7*J7</f>
+        <v>7500</v>
+      </c>
+      <c r="L7" t="str">
+        <f>IF(K7&gt;3000,"Alta",IF(K7&gt;1000,"Media","Baja"))</f>
+        <v>Alta</v>
+      </c>
+      <c r="M7">
+        <f>K7*INDEX(tbl_Comisiones[PCT_comision],MATCH(I7,tbl_Comisiones[Categoria],0))</f>
+        <v>450</v>
+      </c>
+      <c r="N7" t="str">
+        <f>INDEX(tbl_vendedores[Zona],MATCH(D7,tbl_vendedores[Vendedor],0))</f>
+        <v>Norte</v>
+      </c>
+      <c r="O7">
+        <f>HLOOKUP(D7,Catalogos!$E$1:$H$2,2,FALSE)</f>
+        <v>12000</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{56A338E2-FAA5-4BDE-8A62-271F32D614C1}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7" xr:uid="{56A338E2-FAA5-4BDE-8A62-271F32D614C1}">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -3486,13 +3559,13 @@
           <x14:formula1>
             <xm:f>Productos!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H6</xm:sqref>
+          <xm:sqref>H2:H7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{692AEB86-420E-41B6-B0B2-2AD614ECE2C1}">
           <x14:formula1>
             <xm:f>Catalogos!$E$6:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F6</xm:sqref>
+          <xm:sqref>F2:F7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3750,7 +3823,7 @@
       </c>
       <c r="B2" s="2">
         <f>SUM(tbl_Ventas[Total_Ventas])</f>
-        <v>81300</v>
+        <v>88800</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -3780,14 +3853,14 @@
       </c>
       <c r="B3" s="2">
         <f>SUM(tbl_Ventas[Comision])</f>
-        <v>5292</v>
+        <v>5742</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2">
         <f>SUMIF(tbl_Ventas[Categoria],E3,tbl_Ventas[Total_Ventas])</f>
-        <v>67500</v>
+        <v>75000</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -3815,7 +3888,7 @@
       </c>
       <c r="B4" s="2">
         <f>COUNTA(tbl_Ventas[Fecha])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
@@ -3829,11 +3902,11 @@
       </c>
       <c r="J4">
         <f>SUMIF(tbl_Ventas[Vendedor],I4,tbl_Ventas[Total_Ventas])</f>
-        <v>7500</v>
+        <v>15000</v>
       </c>
       <c r="K4">
         <f>SUMIF(tbl_Ventas[Vendedor],I4,tbl_Ventas[Comision])</f>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="L4">
         <f>HLOOKUP(I4,Catalogos!$E$1:$H$2,2,FALSE)</f>
@@ -3841,7 +3914,7 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M5" si="0">IF(J4&gt;L4,"Cumple","No Cumple")</f>
-        <v>No Cumple</v>
+        <v>Cumple</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3850,7 +3923,7 @@
       </c>
       <c r="B5" s="2">
         <f>AVERAGE(tbl_Ventas[Total_Ventas])</f>
-        <v>16260</v>
+        <v>14800</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
@@ -3900,8 +3973,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22DF20C-5319-4F61-AD50-79BACA523E43}">
   <dimension ref="A3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G7"/>
+      <pivotSelection pane="bottomRight" showHeader="1" activeRow="2" click="1" r:id="rId1">
+        <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>